<commit_message>
carnaval foi nada mal
</commit_message>
<xml_diff>
--- a/Lista .xlsx
+++ b/Lista .xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludmi\Google Drive\Mestrado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludmi\Google Drive\Mestrado\Artigo Q-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
-  <si>
-    <t>Chapter 18
-A Q-Learning Approach for Investment
-Decisions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="115">
   <si>
     <t>Autores</t>
   </si>
@@ -50,15 +45,6 @@
     <t>Horel2016</t>
   </si>
   <si>
-    <t>Capítulo de livro, descrição da Teoria do Portfólio e introdução à aplicação de RL q-learning para previsão de retorno de um ativo</t>
-  </si>
-  <si>
-    <t>Relatório breve, traça um paralelo entre RL Model Based e Q-learning</t>
-  </si>
-  <si>
-    <t>RLQL combinado com neuro networks para alocação ótima de ativos</t>
-  </si>
-  <si>
     <t>Neuneier96</t>
   </si>
   <si>
@@ -166,13 +152,7 @@
 Trading Systems and Portfolios</t>
   </si>
   <si>
-    <t>ohn Moody and Matthew Saffell</t>
-  </si>
-  <si>
     <t>Extensão de Moody97 comparando QL com uma tecnica de RL que maximiza a recompensa imediata</t>
-  </si>
-  <si>
-    <t>Moody98</t>
   </si>
   <si>
     <t>Performance Functions and
@@ -235,38 +215,236 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Encontrar Moody97</t>
-  </si>
-  <si>
-    <t>Moody&amp;Saffell</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extensão de Moody97 </t>
   </si>
   <si>
     <t xml:space="preserve"> Gerenciamento de portfólio com RLQL  com análise fatorial utilizando um q-values para cada fator em vez dos ativos</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Lee2001 (encontrar)</t>
-  </si>
-  <si>
     <t>Stock Price Prediction using Reinforcement Learning</t>
   </si>
   <si>
-    <t>Moody2001(encontrar)</t>
-  </si>
-  <si>
     <t>Learning to Trade via Direct Reinforcement. IEEE Transactions on Neural Networks</t>
+  </si>
+  <si>
+    <t>@phdthesis{watkins1989learning, title={Learning from delayed rewards}, author={Watkins, Christopher John Cornish Hellaby}, year={1989}, school={King's College, Cambridge} }</t>
+  </si>
+  <si>
+    <t>{neuneier1996optimal,
+  title={Optimal asset allocation using adaptive dynamic programming},
+  author={Neuneier, Ralph},
+  booktitle={Advances in Neural Information Processing Systems},
+  pages={952--958},
+  year={1996}
+}</t>
+  </si>
+  <si>
+    <t>article{moody2001learning,
+  title={Learning to trade via direct reinforcement},
+  author={Moody, John and Saffell, Matthew},
+  journal={IEEE transactions on neural Networks},
+  volume={12},
+  number={4},
+  pages={875--889},
+  year={2001},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>inproceedings{moody1998reinforcement,
+  title={Reinforcement Learning for Trading Systems and Portfolios.},
+  author={Moody, John E and Saffell, Matthew and Liao, Y and Wu, L},
+  booktitle={KDD},
+  pages={279--283},
+  year={1998}
+}</t>
+  </si>
+  <si>
+    <t>Moody2001</t>
+  </si>
+  <si>
+    <t>John Moody and Matthew Saffell</t>
+  </si>
+  <si>
+    <t>Usa tecnica de Reforço Direto, que se diz melhor que TD-learnint e Qlearning</t>
+  </si>
+  <si>
+    <t>Propõe um sistema de gerenciamento de portfolio (QSR) que usa QL e um algoritmo de maximização do lucro relativo ajustado ao risco (sharpe ratio) com duas redes neurais.</t>
+  </si>
+  <si>
+    <t>@inproceedings{lee2001stock, title={Stock price prediction using reinforcement learning}, author={Lee, Jae Won}, booktitle={Industrial Electronics, 2001. Proceedings. ISIE 2001. IEEE International Symposium on}, volume={1}, pages={690--695}, year={2001}, organization={IEEE} }</t>
+  </si>
+  <si>
+    <t>Jae Won Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lee2001 </t>
+  </si>
+  <si>
+    <t>Utiliza TD-learning para previsão de preços no mercado coreano. Uma rede neural é utilizada para aproximar a função, onde cada estado do sistema markoviano corresponde à tendencia de preço em um dado momento.</t>
+  </si>
+  <si>
+    <t>@inproceedings{lee2002multi, title={A multi-agent Q-learning framework for optimizing stock trading systems}, author={Lee, Jae Won and Jangmin, O}, booktitle={International Conference on Database and Expert Systems Applications}, pages={153--162}, year={2002}, organization={Springer} }</t>
+  </si>
+  <si>
+    <t>@inproceedings{lee2004q, title={A Q-learning based approach to design of intelligent stock trading agents}, author={Lee, JW and Hong, E and Park, J}, booktitle={Engineering Management Conference, 2004. Proceedings. 2004 IEEE International}, volume={3}, pages={1289--1292}, year={2004}, organization={IEEE} }</t>
+  </si>
+  <si>
+    <t>@article{gagliolo2006learning, title={Learning dynamic algorithm portfolios}, author={Gagliolo, Matteo and Schmidhuber, J{\"u}rgen}, journal={Annals of Mathematics and Artificial Intelligence}, volume={47}, number={3-4}, pages={295--328}, year={2006}, publisher={Springer} }</t>
+  </si>
+  <si>
+    <t>bib.tex</t>
+  </si>
+  <si>
+    <t>@inproceedings{li2007independent, title={Independent factor reinforcement learning for portfolio management}, author={Li, Jian and Zhang, Kun and Chan, Laiwan}, booktitle={International Conference on Intelligent Data Engineering and Automated Learning}, pages={1020--1031}, year={2007}, organization={Springer} }</t>
+  </si>
+  <si>
+    <t>@article{lee2007multiagent, title={A Multiagent Approach to $ Q $-Learning for Daily Stock Trading}, author={Lee, Jae Won and Park, Jonghun and Jangmin, O and Lee, Jongwoo and Hong, Euyseok}, journal={IEEE Transactions on Systems, Man, and Cybernetics-Part A: Systems and Humans}, volume={37}, number={6}, pages={864--877}, year={2007}, publisher={IEEE} }</t>
+  </si>
+  <si>
+    <t>Reformulação do trabalho anterior de 2002</t>
+  </si>
+  <si>
+    <t>@article{necchireinforcement, title={Reinforcement Learning For Automated Trading}, author={Necchi, Pierpaolo G} }</t>
+  </si>
+  <si>
+    <t>Desenvolve um algoritmo baseado em RL, Policy Gradient Methods</t>
+  </si>
+  <si>
+    <t>@incollection{varela2016q, title={A q-learning approach for investment decisions}, author={Varela, Mart{\'\i}n and Viera, Omar and Robledo, Franco}, booktitle={Trends in Mathematical Economics}, pages={347--368}, year={2016}, publisher={Springer} }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A Q-Learning Approach for Investment
+Decisions</t>
+  </si>
+  <si>
+    <t>Varela2016</t>
+  </si>
+  <si>
+    <t>Capítulo de livro, descrição da Teoria do Portfólio e introdução à aplicação de RL q-learning para previsão de retorno de um úico ativo</t>
+  </si>
+  <si>
+    <t>@article{horel2016dynamic, title={Dynamic Asset Allocation Using Reinforcement Learning}, author={Horel, Enguerrand and Sarkar, Rahul and Storchan, Victor}, year={2016} }</t>
+  </si>
+  <si>
+    <t>Relatório brev, traça um paralelo entre RL Model Based e Q-learning</t>
+  </si>
+  <si>
+    <t>@article{jiang2017deep, title={A Deep Reinforcement Learning Framework for the Financial Portfolio Management Problem}, author={Jiang, Zhengyao and Xu, Dixing and Liang, Jinjun}, journal={arXiv preprint arXiv:1706.10059}, year={2017} }</t>
+  </si>
+  <si>
+    <t>Esse me parece ser o estado da arte. Artigo extremamente complexo, utilizando convolutional neural networks em um mercado de criptomoedas com séries de 30 minutos.</t>
+  </si>
+  <si>
+    <t>Convergencia do Q-learning</t>
+  </si>
+  <si>
+    <t>Watkins92</t>
+  </si>
+  <si>
+    <t>Technical Note Q-learning</t>
+  </si>
+  <si>
+    <t>Christopher  Watkins e Peter Dayan</t>
+  </si>
+  <si>
+    <t>article{watkins1992q,
+  title={Q-learning},
+  author={Watkins, Christopher JCH and Dayan, Peter},
+  journal={Machine learning},
+  volume={8},
+  number={3-4},
+  pages={279--292},
+  year={1992},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t>Reinforcement learning for trading systems and portfolios: Immediate vs future rewards</t>
+  </si>
+  <si>
+    <t>incollection{moody1998reinforcement,
+  title={Reinforcement learning for trading systems and portfolios: Immediate vs future rewards},
+  author={Moody, John and Saffell, Matthew and Liao, Yuansong and Wu, Lizhong},
+  booktitle={Decision Technologies for Computational Finance},
+  pages={129--140},
+  year={1998},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t>Algorithm Trading using Q-Learning and Recurrent Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>XinDu2016</t>
+  </si>
+  <si>
+    <t>Xin Du Jinjian Zhai</t>
+  </si>
+  <si>
+    <t>article{du2016algorithm,
+  title={Algorithm Trading using Q-Learning and Recurrent Reinforcement Learning},
+  author={Du, Xin and Zhai, Jinjian and Lv, Koupin},
+  journal={positions},
+  volume={1},
+  pages={1},
+  year={2016},
+  publisher={Citeseer}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk-Sensitive Reinforcement Learning
+</t>
+  </si>
+  <si>
+    <t>article{mihatsch2002risk,
+  title={Risk-sensitive reinforcement learning},
+  author={Mihatsch, Oliver and Neuneier, Ralph},
+  journal={Machine learning},
+  volume={49},
+  number={2-3},
+  pages={267--290},
+  year={2002},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t>Neuneier2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mihatsch, Oliver and Neuneier, Ralph </t>
+  </si>
+  <si>
+    <t>inproceedings{gao2000algorithm, title={An algorithm for trading and portfolio management using Q-learning and sharpe ratio maximization}, author={Gao, Xiu and Chan, Laiwan}, booktitle={Proceedings of the international conference on neural information processing}, pages={832--837}, year={2000} }</t>
+  </si>
+  <si>
+    <t>RLQL combinado com neuro networks para alocação ótima de ativos. Compara programação dinâmica e QL com dados sintéticos e faz uma aplicação do QL usando DAX indice de mercado alemão.</t>
+  </si>
+  <si>
+    <t>Usa uma transformação das diferenças temporais (TD) para reformular versoes sensíveis ao risco de algoritmos de RL (Q-learning, TD-learning)</t>
+  </si>
+  <si>
+    <t>Moody98RL</t>
+  </si>
+  <si>
+    <t>Moody98Perf</t>
+  </si>
+  <si>
+    <t>Encontrar Moody98QL</t>
+  </si>
+  <si>
+    <t>voltar aqui</t>
+  </si>
+  <si>
+    <t>encontrar pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,13 +460,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -318,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -330,6 +544,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -646,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC7E835-4272-4313-8880-F23D3252DE14}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,481 +915,647 @@
     <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="44.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="70.26953125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4">
         <v>1989</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1992</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="17" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1996</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1998</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1996</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1998</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="D6" s="4">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4">
         <v>1998</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1998</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1998</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="18" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2001</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="D12" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="17" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2002</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="4" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2004</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2007</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="17" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2007</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="4">
-        <v>2000</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="F16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4">
-        <v>2002</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2007</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2012</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2004</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2007</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2007</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D19" s="12">
+        <v>2015</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="4">
-        <v>2007</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2016</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="17" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2016</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="4">
-        <v>2012</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2015</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="D22" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="14">
         <v>2016</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4">
-        <v>2016</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="4">
-        <v>2017</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2017</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" s="14"/>
+      <c r="F25" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F40">
-    <sortCondition ref="D1"/>
+  <sortState ref="A2:G42">
+    <sortCondition ref="D11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>